<commit_message>
Add nkbblocks stage1 evidence
Add nkbblocks stage1 evidence
</commit_message>
<xml_diff>
--- a/anurg/evidence.xlsx
+++ b/anurg/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahana\Downloads\anurg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F19C7B-597A-4A22-A2FE-6E2CB379CDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F5E574-88D9-4D20-90D3-23B0B0C228D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="49">
   <si>
     <t>TeamName</t>
   </si>
@@ -76,33 +76,15 @@
     <t>ClassID</t>
   </si>
   <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
     <t>nft id</t>
   </si>
   <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
     <t>ibc class on chain</t>
   </si>
   <si>
@@ -143,13 +125,79 @@
   </si>
   <si>
     <t>uptick1swxdrv38n8php20hgdjcdkdvn7atp75uyfdhey</t>
+  </si>
+  <si>
+    <t>anurggon2023</t>
+  </si>
+  <si>
+    <t>BA30B712772D1F8483F8FD5847D9254A8039BD97ABEF800A0A3B027E445CCFA4</t>
+  </si>
+  <si>
+    <t>63D8629C0C780008F49536D5D21B548B67EACED29188587A054B8346B5B69CB4</t>
+  </si>
+  <si>
+    <t>nkb3</t>
+  </si>
+  <si>
+    <t>9924EC5E588EAF53B83A28C1581EDD17D196C2F97C43B4221F667353EB767852</t>
+  </si>
+  <si>
+    <t>nkb2</t>
+  </si>
+  <si>
+    <t>nkb4</t>
+  </si>
+  <si>
+    <t>nkb5</t>
+  </si>
+  <si>
+    <t>nkb6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anurggon2023 </t>
+  </si>
+  <si>
+    <t>481D480BFE98EE07E16789899A2AAB76E0E8672E41848309ADE654C08EC15556</t>
+  </si>
+  <si>
+    <t>2B1ED7E515BBF340F1485AD2A57C2367F983FE9D5AC44C47295636A001E27EA2</t>
+  </si>
+  <si>
+    <t>59FC844ADB0D5FF47182C595608DF74BB0946D6665849911312C7483A12B33DD</t>
+  </si>
+  <si>
+    <t>DB4DAB23801FB4C97EC7223F891D1284A8C71DA466B257B7730015414B348697</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>stars1acjhhuhhhhcmu4ad2ts0dsnw8sh2tgnjxxk2vl92sq6rmkpd7urqk3s4ae</t>
+  </si>
+  <si>
+    <t>FBA3CF39D17ACE60B15C5A2EEFC56CE4FBC095264A6D454AF5FF5D1061A23C09</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>127FDD6B03BD1EAB39FE383DA784A7FA0954A6EB52162F94B7220F2BB7D4CFFA</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>ibc/4D10168A803469578F43912196D6DCFED3DC2BEF397E4C211935CA2FC398DD13</t>
+  </si>
+  <si>
+    <t>E455F3100102F29D042D5DF2C70B0C5AEAB491EF333E248693CD6C109B397F6C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -167,6 +215,29 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF24292F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -195,11 +266,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
@@ -587,28 +667,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -633,15 +713,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -666,15 +746,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -699,15 +779,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -732,15 +812,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -765,25 +845,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -808,25 +888,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -851,25 +931,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -894,25 +974,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -937,25 +1017,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -980,25 +1060,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1011,11 +1091,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="86.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -1028,10 +1111,10 @@
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1056,25 +1139,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1099,25 +1182,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1141,12 +1224,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1176,12 +1259,12 @@
     </row>
     <row r="2" spans="1:1" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1211,12 +1294,12 @@
     </row>
     <row r="2" spans="1:1" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1246,12 +1329,12 @@
     </row>
     <row r="2" spans="1:1" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1266,13 +1349,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" customWidth="1"/>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1284,23 +1370,67 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+      <c r="A2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.25">
+      <c r="A3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14.25">
+      <c r="A4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.25">
+      <c r="A5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14.25">
+      <c r="A6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1308,11 +1438,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="2" width="76.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1324,24 +1456,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1354,7 +1486,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
@@ -1370,24 +1504,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
+      <c r="A2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1400,7 +1534,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
@@ -1416,24 +1552,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
+      <c r="A2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1446,7 +1582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
@@ -1464,29 +1602,29 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+      <c r="A2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1506,15 +1644,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1539,15 +1677,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding after typos corrections in task A5 & A6
</commit_message>
<xml_diff>
--- a/anurg/evidence.xlsx
+++ b/anurg/evidence.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahana\Downloads\anurg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anurag.bhatt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F5E574-88D9-4D20-90D3-23B0B0C228D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="48">
   <si>
     <t>TeamName</t>
   </si>
@@ -184,9 +183,6 @@
     <t>127FDD6B03BD1EAB39FE383DA784A7FA0954A6EB52162F94B7220F2BB7D4CFFA</t>
   </si>
   <si>
-    <t>gon-irishub-1</t>
-  </si>
-  <si>
     <t>ibc/4D10168A803469578F43912196D6DCFED3DC2BEF397E4C211935CA2FC398DD13</t>
   </si>
   <si>
@@ -196,7 +192,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -266,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -279,7 +275,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,7 +617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -698,7 +693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -731,7 +726,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -764,7 +759,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -797,7 +792,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -830,7 +825,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -873,7 +868,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -916,7 +911,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -959,7 +954,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1002,7 +997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1045,7 +1040,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1088,7 +1083,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1124,7 +1119,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1167,7 +1162,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1210,7 +1205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1243,7 +1238,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1278,7 +1273,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1313,7 +1308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1348,7 +1343,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1435,11 +1430,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
@@ -1483,11 +1478,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
@@ -1515,7 +1510,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>30</v>
@@ -1531,11 +1526,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
@@ -1558,9 +1553,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.25">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>42</v>
@@ -1568,8 +1563,8 @@
       <c r="C2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>46</v>
+      <c r="D2" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1579,11 +1574,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
@@ -1613,13 +1608,13 @@
         <v>45</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>46</v>
+      <c r="D2" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1629,7 +1624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1662,7 +1657,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Added Evidences for Tasks A7 - A20
</commit_message>
<xml_diff>
--- a/anurg/evidence.xlsx
+++ b/anurg/evidence.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anurag.bhatt\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahana\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045666DA-EA71-4AE9-9B12-99E398B9DDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="11" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="90">
   <si>
     <t>TeamName</t>
   </si>
@@ -81,21 +82,6 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
   </si>
   <si>
@@ -188,12 +174,153 @@
   <si>
     <t>E455F3100102F29D042D5DF2C70B0C5AEAB491EF333E248693CD6C109B397F6C</t>
   </si>
+  <si>
+    <t>nkb1</t>
+  </si>
+  <si>
+    <t>nkbb7</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>52E5851D3C2633EC67553A6ECC349C9E1D23101EE94CD29CAD817FDDC3A050E5</t>
+  </si>
+  <si>
+    <t>117A0639BE4037B9CA66A835BD07C238616E02878B350056A5AE3A5AED214A69</t>
+  </si>
+  <si>
+    <t>304BFC36BD8E848ED0A65113A66EF49726453AC04AB5402A76F173D9E408D086</t>
+  </si>
+  <si>
+    <t>343FB9E86980DC4BF778C830A2BE5529F515EEC43028FE1F7770BC9A5F1A29B7</t>
+  </si>
+  <si>
+    <t>57CDFF35F03AFA8B1BFBF13B58FA259C21B7322108754801D824C5CE02AF050C</t>
+  </si>
+  <si>
+    <t>0E3296F7FC0D5D37683F0FE06DBD5A82EBD43ED23ECDF9FD9F1FC84DA661E2C8</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>F06D57D8456E2ED378C7B7AA94E83230F03CAB9E99CE3ABF925F8B3325212588</t>
+  </si>
+  <si>
+    <t>C6BB0109570C5F9C03EB43F78DFA01D764B0299D289AC1119FF5D54856E032E1</t>
+  </si>
+  <si>
+    <t>A09CDD9E15BB419EC3FFFABB66EC7629003BA73209CEB167645996745E4A8503</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>DFE880192AFADABF6BCA784DE6DA1B27195496FC5AC3FECC075A97DA9492CA5D</t>
+  </si>
+  <si>
+    <t>0B1A471B6AEA08A081B42AEA274CDA5A3FF7FCC023E75CE2786A09347F7BD88B </t>
+  </si>
+  <si>
+    <t>A61656056C14BF51C7B55C4D8C4B7E53465C4D22FA36A5A99DAEDD8276F2F67C </t>
+  </si>
+  <si>
+    <t>8F63CB4A2AE4FF41A8EC65824339FB7CDF076BBCA5A7191F220F59D7AA72D316</t>
+  </si>
+  <si>
+    <t>F0BFF99784D9C3DBC57E6E9F25D05231B61B3F74C898BD20D574DE9870F5A98A</t>
+  </si>
+  <si>
+    <t>9D38B779C9C037BA72884152348D6AC52324BE8AD908A3758D0631631B1E1F84</t>
+  </si>
+  <si>
+    <t>967855897C740C03314692B64BBB04C1ECA28CC95D1D34A21949A6A48BC1C500</t>
+  </si>
+  <si>
+    <t>F71223E4D93943C78CB87BC0B9F4EEF855A112F3A2B9D818A1B4DF28077B81FA</t>
+  </si>
+  <si>
+    <t>3C62F2C8C1771FC505FAC0CB5AA305B4D3D153080ABF70BA690E0D36915B4C66</t>
+  </si>
+  <si>
+    <t>CF0239EFD1AB5E76F2FC2A6D3FA6B4B033DEA63FA49261D448C68DDC5D90C3DE</t>
+  </si>
+  <si>
+    <t>9DAD2EC24391BF7EC790F88FEB0F5BD4C7E7FC692341A442785717CBB966BC3F</t>
+  </si>
+  <si>
+    <t>77A003FCF63BD647E3078BC71CAE6C1F34EA2CFE3F5F671B63F9D164BD72B552</t>
+  </si>
+  <si>
+    <t>7478BD4B09A04AA92A4B82D75A74983301EB7CC33E6B4BAD03EDBC0FCA0048B7</t>
+  </si>
+  <si>
+    <t>ACB407F68144F4B621DC2D427774055BBA5C1FB6683EB85096A8CA7DBEA20BA3</t>
+  </si>
+  <si>
+    <t>DA15A9938D7A06F4E936AE89DA62427343B78DDE7F161ABF70F4217C438ECA10</t>
+  </si>
+  <si>
+    <t>A35542DB5582CCEAA9EE8ECC6AAE5DC94EF4C8FEFF5793E16F62388521E1A1C9 </t>
+  </si>
+  <si>
+    <t>CBB2AAE5E42A685D3E4D52F497902359BF76908E83FAFE3FA3E6459BD5BA3AD6</t>
+  </si>
+  <si>
+    <t>8FC4BC1EED71760327334F5F751A33D4D6317CC2157758153D6DD85FA17D90F9</t>
+  </si>
+  <si>
+    <t>411A5C002BB1CA0595B5ABDF8C67D5733E285F0B7160946FA2EA98C3CBA58474</t>
+  </si>
+  <si>
+    <t>F21681C0FF923E7F05AFBF679D3752ABAAEB53506E5412C83AEE63CBB28E85A2 </t>
+  </si>
+  <si>
+    <t>F8B515655278CEE4225776788D04D6B96DFE46C6501F1841146C29A55CB5D947</t>
+  </si>
+  <si>
+    <t>A6136571012451A8F6554E66B09AE5B49E7A42A817D790DCF1FC9FBF59ED0DCB</t>
+  </si>
+  <si>
+    <t>4295C0FAF164FB8AE50DB8F472640DF8A080FFF9FE7324A446B032160A729C0F</t>
+  </si>
+  <si>
+    <t>CD778B4C77229EA01CCC6DA725C1EF983DA44B51172B224A38C7B854E5F1B83A</t>
+  </si>
+  <si>
+    <t>4923B79BCB38D90B7AE1537C0DF4DE21D7E1013098403E6532E571E6F42FB79B</t>
+  </si>
+  <si>
+    <t>23997DC8AC84CC9DA6F2B64D56235916F59F00EA20AB88F92934B4857DC66083</t>
+  </si>
+  <si>
+    <t>B79A61245817135BAD503628C175856FFB2FB814C69E4D9916C0ECA511DA3D1C</t>
+  </si>
+  <si>
+    <t>ibc/9E8B20AFE0250E731F776CB486D58F992DA9F13F7741448D2A0CBBDC5BFB5CD6</t>
+  </si>
+  <si>
+    <t>ibc/066470B87B0893263CDA5748B181D44F5F041FF95E2AFABB03020FB8FCD1FAF5</t>
+  </si>
+  <si>
+    <t>ibc/390E7744446BDFEA46B281507C25964C17766CA9FF15F9B43D198091E35144AC</t>
+  </si>
+  <si>
+    <t>ibc/FAF3370617C1E1AB1A6A0B1D6ECC68E8FFBF20D5910FA697D2BAE44DB85C2070</t>
+  </si>
+  <si>
+    <t>ibc/90CC5D46A6876DF7EA00683F963ED803D59A9D87AF4C3978DBD27C17412C219C</t>
+  </si>
+  <si>
+    <t>ibc/B9D3B075121B75AD5260F80C9B3A9FE431C19A05787A82B8C80A4E8CBA2B762D</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -235,6 +362,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292F"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -262,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -275,6 +408,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,7 +753,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -662,28 +798,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -693,14 +829,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="84.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -712,11 +850,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
+      <c r="A2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -726,14 +864,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="77.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -745,11 +885,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
+      <c r="A2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -759,14 +899,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="99.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -778,11 +920,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
+      <c r="A2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -792,14 +934,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="97.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -810,12 +954,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
+    <row r="2" spans="1:2" ht="17.25">
+      <c r="A2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -825,14 +969,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="92.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -843,22 +989,36 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
+    <row r="2" spans="1:2" ht="17.25">
+      <c r="A2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25">
+      <c r="A3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25">
+      <c r="A4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25">
+      <c r="A5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -868,14 +1028,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="72.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -886,22 +1048,36 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
+    <row r="2" spans="1:2" ht="17.25">
+      <c r="A2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25">
+      <c r="A3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25">
+      <c r="A4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25">
+      <c r="A5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -911,14 +1087,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="79.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -929,23 +1107,40 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
-      </c>
+    <row r="2" spans="1:2" ht="17.25">
+      <c r="A2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25">
+      <c r="A3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25">
+      <c r="A4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25">
+      <c r="A5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25">
+      <c r="B6" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -954,14 +1149,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="90" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -972,22 +1169,36 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
+    <row r="2" spans="1:2" ht="17.25">
+      <c r="A2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25">
+      <c r="A3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25">
+      <c r="A4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25">
+      <c r="A5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -997,14 +1208,16 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="84.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -1015,22 +1228,36 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
+    <row r="2" spans="1:2" ht="17.25">
+      <c r="A2" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25">
+      <c r="A3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25">
+      <c r="A4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25">
+      <c r="A5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1040,14 +1267,16 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="110.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -1058,22 +1287,36 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
+    <row r="2" spans="1:2" ht="17.25">
+      <c r="A2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25">
+      <c r="A3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25">
+      <c r="A4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25">
+      <c r="A5" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1083,7 +1326,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1106,10 +1349,10 @@
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1119,14 +1362,16 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="102.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -1137,22 +1382,52 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
+    <row r="2" spans="1:2" ht="17.25">
+      <c r="A2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25">
+      <c r="A3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25">
+      <c r="A4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25">
+      <c r="A5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25">
+      <c r="A6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25">
+      <c r="A7" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1162,14 +1437,16 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="89" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -1180,22 +1457,52 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
+    <row r="2" spans="1:2" ht="17.25">
+      <c r="A2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25">
+      <c r="A3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25">
+      <c r="A4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25">
+      <c r="A5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25">
+      <c r="A6" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25">
+      <c r="A7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1205,7 +1512,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1219,12 +1526,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1238,7 +1545,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1254,12 +1561,12 @@
     </row>
     <row r="2" spans="1:1" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1273,7 +1580,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1289,12 +1596,12 @@
     </row>
     <row r="2" spans="1:1" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1308,7 +1615,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1324,12 +1631,12 @@
     </row>
     <row r="2" spans="1:1" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1343,7 +1650,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1370,57 +1677,57 @@
     </row>
     <row r="2" spans="1:3" ht="14.25">
       <c r="A2" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25">
       <c r="A3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25">
       <c r="A4" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25">
       <c r="A5" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25">
       <c r="A6" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1430,7 +1737,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1459,16 +1766,16 @@
     </row>
     <row r="2" spans="1:4" ht="15">
       <c r="A2" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1478,7 +1785,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1507,16 +1814,16 @@
     </row>
     <row r="2" spans="1:4" ht="14.25">
       <c r="A2" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1526,7 +1833,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1555,16 +1862,16 @@
     </row>
     <row r="2" spans="1:4" ht="15">
       <c r="A2" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1574,10 +1881,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1605,16 +1912,16 @@
     </row>
     <row r="2" spans="1:4" ht="14.25">
       <c r="A2" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1624,14 +1931,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="66.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -1642,29 +1951,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
+    <row r="2" spans="1:2" ht="17.25">
+      <c r="A2" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="89" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -1675,13 +1986,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
+    <row r="2" spans="1:2" ht="17.25">
+      <c r="A2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Made some corrections in Sheet A18
</commit_message>
<xml_diff>
--- a/anurg/evidence.xlsx
+++ b/anurg/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahana\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045666DA-EA71-4AE9-9B12-99E398B9DDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E49249-871B-4FDB-AEED-02D483D07FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="11" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -1032,7 +1032,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
@@ -1270,13 +1270,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="110.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
@@ -1300,7 +1301,7 @@
         <v>69</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25">
@@ -1316,7 +1317,7 @@
         <v>71</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1440,7 +1441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1654,7 +1655,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Added evidence for B1/B2
</commit_message>
<xml_diff>
--- a/anurg/evidence.xlsx
+++ b/anurg/evidence.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahana\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anurag.bhatt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E49249-871B-4FDB-AEED-02D483D07FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" tabRatio="500" firstSheet="14" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="94">
   <si>
     <t>TeamName</t>
   </si>
@@ -315,11 +314,23 @@
   <si>
     <t>ibc/B9D3B075121B75AD5260F80C9B3A9FE431C19A05787A82B8C80A4E8CBA2B762D</t>
   </si>
+  <si>
+    <t>C65AE751D993685B15C329EF260E26050F1B3A6677A1837F339FF494B49186DB</t>
+  </si>
+  <si>
+    <t>51D9F476FA2BCCBB4B25F7C34448D1582EADCFFD5C7923F58263F9CC71A6E8AD</t>
+  </si>
+  <si>
+    <t>A32CCBD12E289418427069C7C369DBD81232D0619C7A4AB95B391214E18F296F</t>
+  </si>
+  <si>
+    <t>77B8533C4CFA45E30A68E404C68ED42C5A015AEEC13AE2F9BBD1F1354BA277BF</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8">
     <font>
       <sz val="10"/>
@@ -753,7 +764,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -829,7 +840,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -864,7 +875,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -899,7 +910,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -934,7 +945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -969,7 +980,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1028,7 +1039,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1087,7 +1098,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1149,7 +1160,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1208,7 +1219,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1267,10 +1278,10 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1327,7 +1338,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1363,7 +1374,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1438,7 +1449,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1513,10 +1524,12 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <sheetData>
@@ -1526,13 +1539,48 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
+      <c r="A2" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="14.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="14.25">
+      <c r="A2" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="14.25">
+      <c r="A3" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1545,12 +1593,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1580,12 +1628,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1615,43 +1663,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="14.25">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="14.25">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="14.25">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1738,7 +1751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1786,7 +1799,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1834,7 +1847,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1882,7 +1895,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1932,7 +1945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1967,7 +1980,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Added Evidence for B5-B7
</commit_message>
<xml_diff>
--- a/anurg/evidence.xlsx
+++ b/anurg/evidence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" tabRatio="500" firstSheet="14" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" tabRatio="500" firstSheet="15" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -37,13 +37,14 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="98">
   <si>
     <t>TeamName</t>
   </si>
@@ -81,12 +82,6 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>nkbblocks</t>
   </si>
   <si>
@@ -325,13 +320,31 @@
   </si>
   <si>
     <t>77B8533C4CFA45E30A68E404C68ED42C5A015AEEC13AE2F9BBD1F1354BA277BF</t>
+  </si>
+  <si>
+    <t>C34269944C8891F2A7398E47D91268601E75162D4A5721FD1844B190E2056C2C</t>
+  </si>
+  <si>
+    <t>5D03F1BA609141A667F5B88380249004558534380A404E85AA3E6DE44506BB5C</t>
+  </si>
+  <si>
+    <t>AC0E146D87A6D0668E1A5FB945674D5EFC345E27D957DF55126491D1B146290C</t>
+  </si>
+  <si>
+    <t>A433A24F0AA894444FE3F86C534380E3865EDFC29A57EC304EBE18297246F1BE</t>
+  </si>
+  <si>
+    <t>2ACCF0BAA35DAFB135D9CB6573EB6EC7C8F247110EBD64581276D2DF5EDF2FEC</t>
+  </si>
+  <si>
+    <t>C261AD00573015FCAAE97896C08B0B03FC038C9AD9FBE4D4D17DBE45726B3826</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -379,8 +392,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,8 +411,14 @@
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAFAFC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -402,11 +426,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFEBE9F1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -422,6 +455,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,28 +846,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -862,10 +899,10 @@
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -897,10 +934,10 @@
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -932,10 +969,10 @@
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -967,10 +1004,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25">
       <c r="A2" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1002,34 +1039,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25">
       <c r="A2" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25">
       <c r="A5" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1061,34 +1098,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25">
       <c r="A2" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25">
       <c r="A3" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25">
       <c r="A4" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25">
       <c r="A5" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1120,34 +1157,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25">
       <c r="A2" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25">
       <c r="A3" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25">
       <c r="A4" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25">
       <c r="A5" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25">
@@ -1182,34 +1219,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25">
       <c r="A2" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25">
       <c r="A3" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25">
       <c r="A4" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25">
       <c r="A5" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1241,34 +1278,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25">
       <c r="A2" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25">
       <c r="A3" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25">
       <c r="A4" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25">
       <c r="A5" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1301,34 +1338,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25">
       <c r="A2" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25">
       <c r="A3" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25">
       <c r="A4" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25">
       <c r="A5" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1361,10 +1398,10 @@
     </row>
     <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1396,50 +1433,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25">
       <c r="A2" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25">
       <c r="A3" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25">
       <c r="A4" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25">
       <c r="A5" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25">
       <c r="A6" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25">
       <c r="A7" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1471,50 +1508,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25">
       <c r="A2" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25">
       <c r="A3" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25">
       <c r="A4" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25">
       <c r="A5" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25">
       <c r="A6" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25">
       <c r="A7" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1527,7 +1564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1540,12 +1577,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1575,12 +1612,12 @@
     </row>
     <row r="2" spans="1:1" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1598,7 +1635,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1609,13 +1646,48 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="14.25">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
+      <c r="A2" s="11" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="14.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="14.25">
+      <c r="A2" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="14.25">
+      <c r="A3" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1628,38 +1700,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="14.25">
+    <row r="1" spans="1:1" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="14.25">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
+      <c r="A2" s="12" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
-  </headerFooter>
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1691,57 +1758,57 @@
     </row>
     <row r="2" spans="1:3" ht="14.25">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25">
       <c r="A4" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25">
       <c r="A5" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25">
       <c r="A6" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1780,16 +1847,16 @@
     </row>
     <row r="2" spans="1:4" ht="15">
       <c r="A2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1828,16 +1895,16 @@
     </row>
     <row r="2" spans="1:4" ht="14.25">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1876,16 +1943,16 @@
     </row>
     <row r="2" spans="1:4" ht="15">
       <c r="A2" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1926,16 +1993,16 @@
     </row>
     <row r="2" spans="1:4" ht="14.25">
       <c r="A2" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1967,10 +2034,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25">
       <c r="A2" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2002,10 +2069,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25">
       <c r="A2" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2">

</xml_diff>